<commit_message>
Instruction ADDU working, developed  h+cpp  for instr API
</commit_message>
<xml_diff>
--- a/Instruction List.xlsx
+++ b/Instruction List.xlsx
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,7 +826,8 @@
     <col min="4" max="4" width="22.7265625" customWidth="1"/>
     <col min="7" max="7" width="22.453125" customWidth="1"/>
     <col min="8" max="8" width="26.08984375" customWidth="1"/>
-    <col min="10" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.54296875" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -891,8 +892,10 @@
 </v>
       </c>
       <c r="K3" t="str">
-        <f>CONCATENATE("case ", H3,  ": return ", C3, " (state, ", IF(F3="I", "rs, rt, imm", IF(F3="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 33: return ADDU (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H3, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C3,CHAR(34), "\n",");}",CHAR(10),"return ",C3," (state, ",IF(F3="I","rs, rt, imm",IF(F3="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 33:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ADDU"\n);}
+return ADDU (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>136</v>
@@ -927,8 +930,10 @@
 </v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE("case ", H4,  ": return ", C4, " (state, ", IF(F4="I", "rs, rt, imm", IF(F4="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 35: return SUBU (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H4, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C4,CHAR(34), "\n",");}",CHAR(10),"return ",C4," (state, ",IF(F4="I","rs, rt, imm",IF(F4="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 35:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SUBU"\n);}
+return SUBU (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>136</v>
@@ -963,8 +968,10 @@
 </v>
       </c>
       <c r="K5" t="str">
-        <f>CONCATENATE("case ", H5,  ": return ", C5, " (state, ", IF(F5="I", "rs, rt, imm", IF(F5="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 36: return AND (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H5, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C5,CHAR(34), "\n",");}",CHAR(10),"return ",C5," (state, ",IF(F5="I","rs, rt, imm",IF(F5="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 36:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "AND"\n);}
+return AND (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>136</v>
@@ -999,8 +1006,10 @@
 </v>
       </c>
       <c r="K6" t="str">
-        <f>CONCATENATE("case ", H6,  ": return ", C6, " (state, ", IF(F6="I", "rs, rt, imm", IF(F6="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 37: return OR (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H6, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C6,CHAR(34), "\n",");}",CHAR(10),"return ",C6," (state, ",IF(F6="I","rs, rt, imm",IF(F6="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 37:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "OR"\n);}
+return OR (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>136</v>
@@ -1035,8 +1044,10 @@
 </v>
       </c>
       <c r="K7" t="str">
-        <f>CONCATENATE("case ", H7,  ": return ", C7, " (state, ", IF(F7="I", "rs, rt, imm", IF(F7="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 38: return XOR (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H7, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C7,CHAR(34), "\n",");}",CHAR(10),"return ",C7," (state, ",IF(F7="I","rs, rt, imm",IF(F7="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 38:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "XOR"\n);}
+return XOR (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>136</v>
@@ -1071,8 +1082,10 @@
 </v>
       </c>
       <c r="K8" t="str">
-        <f>CONCATENATE("case ", H8,  ": return ", C8, " (state, ", IF(F8="I", "rs, rt, imm", IF(F8="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 43: return SLTU (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H8, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C8,CHAR(34), "\n",");}",CHAR(10),"return ",C8," (state, ",IF(F8="I","rs, rt, imm",IF(F8="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 43:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLTU"\n);}
+return SLTU (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>136</v>
@@ -1107,8 +1120,10 @@
 </v>
       </c>
       <c r="K9" t="str">
-        <f>CONCATENATE("case ", H9,  ": return ", C9, " (state, ", IF(F9="I", "rs, rt, imm", IF(F9="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 8: return ADDI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H9, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C9,CHAR(34), "\n",");}",CHAR(10),"return ",C9," (state, ",IF(F9="I","rs, rt, imm",IF(F9="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 8:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ADDI"\n);}
+return ADDI (state, rs, rt, imm);</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>136</v>
@@ -1143,8 +1158,10 @@
 </v>
       </c>
       <c r="K10" t="str">
-        <f>CONCATENATE("case ", H10,  ": return ", C10, " (state, ", IF(F10="I", "rs, rt, imm", IF(F10="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 9: return ADDIU (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H10, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C10,CHAR(34), "\n",");}",CHAR(10),"return ",C10," (state, ",IF(F10="I","rs, rt, imm",IF(F10="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 9:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ADDIU"\n);}
+return ADDIU (state, rs, rt, imm);</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>136</v>
@@ -1179,8 +1196,10 @@
 </v>
       </c>
       <c r="K11" t="str">
-        <f>CONCATENATE("case ", H11,  ": return ", C11, " (state, ", IF(F11="I", "rs, rt, imm", IF(F11="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 12: return ANDI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H11, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C11,CHAR(34), "\n",");}",CHAR(10),"return ",C11," (state, ",IF(F11="I","rs, rt, imm",IF(F11="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 12:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ANDI"\n);}
+return ANDI (state, rs, rt, imm);</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>136</v>
@@ -1215,8 +1234,10 @@
 </v>
       </c>
       <c r="K12" t="str">
-        <f>CONCATENATE("case ", H12,  ": return ", C12, " (state, ", IF(F12="I", "rs, rt, imm", IF(F12="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 13: return ORI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H12, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C12,CHAR(34), "\n",");}",CHAR(10),"return ",C12," (state, ",IF(F12="I","rs, rt, imm",IF(F12="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 13:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ORI"\n);}
+return ORI (state, rs, rt, imm);</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>136</v>
@@ -1251,8 +1272,10 @@
 </v>
       </c>
       <c r="K13" t="str">
-        <f>CONCATENATE("case ", H13,  ": return ", C13, " (state, ", IF(F13="I", "rs, rt, imm", IF(F13="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 14: return XORI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H13, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C13,CHAR(34), "\n",");}",CHAR(10),"return ",C13," (state, ",IF(F13="I","rs, rt, imm",IF(F13="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 14:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "XORI"\n);}
+return XORI (state, rs, rt, imm);</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>136</v>
@@ -1287,8 +1310,10 @@
 </v>
       </c>
       <c r="K14" t="str">
-        <f>CONCATENATE("case ", H14,  ": return ", C14, " (state, ", IF(F14="I", "rs, rt, imm", IF(F14="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 15: return LUI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H14, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C14,CHAR(34), "\n",");}",CHAR(10),"return ",C14," (state, ",IF(F14="I","rs, rt, imm",IF(F14="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 15:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LUI"\n);}
+return LUI (state, rs, rt, imm);</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>136</v>
@@ -1323,8 +1348,10 @@
 </v>
       </c>
       <c r="K15" t="str">
-        <f>CONCATENATE("case ", H15,  ": return ", C15, " (state, ", IF(F15="I", "rs, rt, imm", IF(F15="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 35: return LW (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H15, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C15,CHAR(34), "\n",");}",CHAR(10),"return ",C15," (state, ",IF(F15="I","rs, rt, imm",IF(F15="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 35:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LW"\n);}
+return LW (state, rs, rt, imm);</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>136</v>
@@ -1359,8 +1386,10 @@
 </v>
       </c>
       <c r="K16" t="str">
-        <f>CONCATENATE("case ", H16,  ": return ", C16, " (state, ", IF(F16="I", "rs, rt, imm", IF(F16="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 43: return SW (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H16, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C16,CHAR(34), "\n",");}",CHAR(10),"return ",C16," (state, ",IF(F16="I","rs, rt, imm",IF(F16="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 43:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SW"\n);}
+return SW (state, rs, rt, imm);</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>136</v>
@@ -1395,8 +1424,10 @@
 </v>
       </c>
       <c r="K17" t="str">
-        <f>CONCATENATE("case ", H17,  ": return ", C17, " (state, ", IF(F17="I", "rs, rt, imm", IF(F17="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 0: return SLL (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H17, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C17,CHAR(34), "\n",");}",CHAR(10),"return ",C17," (state, ",IF(F17="I","rs, rt, imm",IF(F17="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 0:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLL"\n);}
+return SLL (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>136</v>
@@ -1431,8 +1462,10 @@
 </v>
       </c>
       <c r="K18" t="str">
-        <f>CONCATENATE("case ", H18,  ": return ", C18, " (state, ", IF(F18="I", "rs, rt, imm", IF(F18="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 2: return SRL (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H18, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C18,CHAR(34), "\n",");}",CHAR(10),"return ",C18," (state, ",IF(F18="I","rs, rt, imm",IF(F18="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 2:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SRL"\n);}
+return SRL (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>136</v>
@@ -1467,8 +1500,10 @@
 </v>
       </c>
       <c r="K19" t="str">
-        <f>CONCATENATE("case ", H19,  ": return ", C19, " (state, ", IF(F19="I", "rs, rt, imm", IF(F19="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 3: return SRA (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H19, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C19,CHAR(34), "\n",");}",CHAR(10),"return ",C19," (state, ",IF(F19="I","rs, rt, imm",IF(F19="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 3:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SRA"\n);}
+return SRA (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>136</v>
@@ -1503,8 +1538,10 @@
 </v>
       </c>
       <c r="K20" t="str">
-        <f>CONCATENATE("case ", H20,  ": return ", C20, " (state, ", IF(F20="I", "rs, rt, imm", IF(F20="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 6: return SRLV (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H20, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C20,CHAR(34), "\n",");}",CHAR(10),"return ",C20," (state, ",IF(F20="I","rs, rt, imm",IF(F20="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 6:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SRLV"\n);}
+return SRLV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>136</v>
@@ -1539,8 +1576,10 @@
 </v>
       </c>
       <c r="K21" t="str">
-        <f>CONCATENATE("case ", H21,  ": return ", C21, " (state, ", IF(F21="I", "rs, rt, imm", IF(F21="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 7: return SRAV (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H21, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C21,CHAR(34), "\n",");}",CHAR(10),"return ",C21," (state, ",IF(F21="I","rs, rt, imm",IF(F21="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 7:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SRAV"\n);}
+return SRAV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>136</v>
@@ -1575,8 +1614,10 @@
 </v>
       </c>
       <c r="K22" t="str">
-        <f>CONCATENATE("case ", H22,  ": return ", C22, " (state, ", IF(F22="I", "rs, rt, imm", IF(F22="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 32: return ADD (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H22, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C22,CHAR(34), "\n",");}",CHAR(10),"return ",C22," (state, ",IF(F22="I","rs, rt, imm",IF(F22="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 32:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "ADD"\n);}
+return ADD (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>136</v>
@@ -1611,8 +1652,10 @@
 </v>
       </c>
       <c r="K23" t="str">
-        <f>CONCATENATE("case ", H23,  ": return ", C23, " (state, ", IF(F23="I", "rs, rt, imm", IF(F23="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 34: return SUB (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H23, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C23,CHAR(34), "\n",");}",CHAR(10),"return ",C23," (state, ",IF(F23="I","rs, rt, imm",IF(F23="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 34:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SUB"\n);}
+return SUB (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>136</v>
@@ -1647,8 +1690,10 @@
 </v>
       </c>
       <c r="K24" t="str">
-        <f>CONCATENATE("case ", H24,  ": return ", C24, " (state, ", IF(F24="I", "rs, rt, imm", IF(F24="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 42: return SLT (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H24, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C24,CHAR(34), "\n",");}",CHAR(10),"return ",C24," (state, ",IF(F24="I","rs, rt, imm",IF(F24="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 42:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLT"\n);}
+return SLT (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>136</v>
@@ -1683,8 +1728,10 @@
 </v>
       </c>
       <c r="K25" t="str">
-        <f>CONCATENATE("case ", H25,  ": return ", C25, " (state, ", IF(F25="I", "rs, rt, imm", IF(F25="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 4: return SLLV (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H25, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C25,CHAR(34), "\n",");}",CHAR(10),"return ",C25," (state, ",IF(F25="I","rs, rt, imm",IF(F25="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 4:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLLV"\n);}
+return SLLV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>136</v>
@@ -1721,8 +1768,10 @@
 </v>
       </c>
       <c r="K26" t="str">
-        <f>CONCATENATE("case ", H26,  ": return ", C26, " (state, ", IF(F26="I", "rs, rt, imm", IF(F26="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 1: return BLTZ (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H26, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C26,CHAR(34), "\n",");}",CHAR(10),"return ",C26," (state, ",IF(F26="I","rs, rt, imm",IF(F26="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 1:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BLTZ"\n);}
+return BLTZ (state, rs, rt, imm);</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>136</v>
@@ -1759,8 +1808,10 @@
 </v>
       </c>
       <c r="K27" t="str">
-        <f>CONCATENATE("case ", H27,  ": return ", C27, " (state, ", IF(F27="I", "rs, rt, imm", IF(F27="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 1: return BGEZ (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H27, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C27,CHAR(34), "\n",");}",CHAR(10),"return ",C27," (state, ",IF(F27="I","rs, rt, imm",IF(F27="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 1:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BGEZ"\n);}
+return BGEZ (state, rs, rt, imm);</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>136</v>
@@ -1795,8 +1846,10 @@
 </v>
       </c>
       <c r="K28" t="str">
-        <f>CONCATENATE("case ", H28,  ": return ", C28, " (state, ", IF(F28="I", "rs, rt, imm", IF(F28="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 4: return BEQ (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H28, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C28,CHAR(34), "\n",");}",CHAR(10),"return ",C28," (state, ",IF(F28="I","rs, rt, imm",IF(F28="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 4:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BEQ"\n);}
+return BEQ (state, rs, rt, imm);</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>136</v>
@@ -1831,8 +1884,10 @@
 </v>
       </c>
       <c r="K29" t="str">
-        <f>CONCATENATE("case ", H29,  ": return ", C29, " (state, ", IF(F29="I", "rs, rt, imm", IF(F29="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 5: return BNE (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H29, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C29,CHAR(34), "\n",");}",CHAR(10),"return ",C29," (state, ",IF(F29="I","rs, rt, imm",IF(F29="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 5:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BNE"\n);}
+return BNE (state, rs, rt, imm);</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>136</v>
@@ -1867,8 +1922,10 @@
 </v>
       </c>
       <c r="K30" t="str">
-        <f>CONCATENATE("case ", H30,  ": return ", C30, " (state, ", IF(F30="I", "rs, rt, imm", IF(F30="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 6: return BLEZ (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H30, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C30,CHAR(34), "\n",");}",CHAR(10),"return ",C30," (state, ",IF(F30="I","rs, rt, imm",IF(F30="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 6:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BLEZ"\n);}
+return BLEZ (state, rs, rt, imm);</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>136</v>
@@ -1903,8 +1960,10 @@
 </v>
       </c>
       <c r="K31" t="str">
-        <f>CONCATENATE("case ", H31,  ": return ", C31, " (state, ", IF(F31="I", "rs, rt, imm", IF(F31="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 7: return BGTZ (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H31, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C31,CHAR(34), "\n",");}",CHAR(10),"return ",C31," (state, ",IF(F31="I","rs, rt, imm",IF(F31="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 7:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BGTZ"\n);}
+return BGTZ (state, rs, rt, imm);</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>136</v>
@@ -1939,8 +1998,10 @@
 </v>
       </c>
       <c r="K32" t="str">
-        <f>CONCATENATE("case ", H32,  ": return ", C32, " (state, ", IF(F32="I", "rs, rt, imm", IF(F32="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 10: return SLTI (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H32, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C32,CHAR(34), "\n",");}",CHAR(10),"return ",C32," (state, ",IF(F32="I","rs, rt, imm",IF(F32="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 10:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLTI"\n);}
+return SLTI (state, rs, rt, imm);</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>136</v>
@@ -1975,8 +2036,10 @@
 </v>
       </c>
       <c r="K33" t="str">
-        <f>CONCATENATE("case ", H33,  ": return ", C33, " (state, ", IF(F33="I", "rs, rt, imm", IF(F33="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 11: return SLTIU (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H33, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C33,CHAR(34), "\n",");}",CHAR(10),"return ",C33," (state, ",IF(F33="I","rs, rt, imm",IF(F33="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 11:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLTIU"\n);}
+return SLTIU (state, rs, rt, imm);</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>136</v>
@@ -2011,8 +2074,10 @@
 </v>
       </c>
       <c r="K34" t="str">
-        <f>CONCATENATE("case ", H34,  ": return ", C34, " (state, ", IF(F34="I", "rs, rt, imm", IF(F34="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 32: return LB (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H34, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C34,CHAR(34), "\n",");}",CHAR(10),"return ",C34," (state, ",IF(F34="I","rs, rt, imm",IF(F34="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 32:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LB"\n);}
+return LB (state, rs, rt, imm);</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>136</v>
@@ -2047,8 +2112,10 @@
 </v>
       </c>
       <c r="K35" t="str">
-        <f>CONCATENATE("case ", H35,  ": return ", C35, " (state, ", IF(F35="I", "rs, rt, imm", IF(F35="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 33: return LH (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H35, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C35,CHAR(34), "\n",");}",CHAR(10),"return ",C35," (state, ",IF(F35="I","rs, rt, imm",IF(F35="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 33:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LH"\n);}
+return LH (state, rs, rt, imm);</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>136</v>
@@ -2083,8 +2150,10 @@
 </v>
       </c>
       <c r="K36" t="str">
-        <f>CONCATENATE("case ", H36,  ": return ", C36, " (state, ", IF(F36="I", "rs, rt, imm", IF(F36="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 36: return LBU (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H36, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C36,CHAR(34), "\n",");}",CHAR(10),"return ",C36," (state, ",IF(F36="I","rs, rt, imm",IF(F36="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 36:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LBU"\n);}
+return LBU (state, rs, rt, imm);</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>136</v>
@@ -2119,8 +2188,10 @@
 </v>
       </c>
       <c r="K37" t="str">
-        <f>CONCATENATE("case ", H37,  ": return ", C37, " (state, ", IF(F37="I", "rs, rt, imm", IF(F37="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 37: return LHU (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H37, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C37,CHAR(34), "\n",");}",CHAR(10),"return ",C37," (state, ",IF(F37="I","rs, rt, imm",IF(F37="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 37:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LHU"\n);}
+return LHU (state, rs, rt, imm);</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>136</v>
@@ -2155,8 +2226,10 @@
 </v>
       </c>
       <c r="K38" t="str">
-        <f>CONCATENATE("case ", H38,  ": return ", C38, " (state, ", IF(F38="I", "rs, rt, imm", IF(F38="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 40: return SB (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H38, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C38,CHAR(34), "\n",");}",CHAR(10),"return ",C38," (state, ",IF(F38="I","rs, rt, imm",IF(F38="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 40:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SB"\n);}
+return SB (state, rs, rt, imm);</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>136</v>
@@ -2191,8 +2264,10 @@
 </v>
       </c>
       <c r="K39" t="str">
-        <f>CONCATENATE("case ", H39,  ": return ", C39, " (state, ", IF(F39="I", "rs, rt, imm", IF(F39="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 41: return SH (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H39, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C39,CHAR(34), "\n",");}",CHAR(10),"return ",C39," (state, ",IF(F39="I","rs, rt, imm",IF(F39="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 41:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SH"\n);}
+return SH (state, rs, rt, imm);</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>136</v>
@@ -2227,8 +2302,10 @@
 </v>
       </c>
       <c r="K40" t="str">
-        <f>CONCATENATE("case ", H40,  ": return ", C40, " (state, ", IF(F40="I", "rs, rt, imm", IF(F40="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 2: return J (state,  target);</v>
+        <f>CONCATENATE("case ",H40, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C40,CHAR(34), "\n",");}",CHAR(10),"return ",C40," (state, ",IF(F40="I","rs, rt, imm",IF(F40="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 2:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "J"\n);}
+return J (state,  target);</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>136</v>
@@ -2263,8 +2340,10 @@
 </v>
       </c>
       <c r="K41" t="str">
-        <f>CONCATENATE("case ", H41,  ": return ", C41, " (state, ", IF(F41="I", "rs, rt, imm", IF(F41="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 8: return JR (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H41, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C41,CHAR(34), "\n",");}",CHAR(10),"return ",C41," (state, ",IF(F41="I","rs, rt, imm",IF(F41="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 8:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "JR"\n);}
+return JR (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>136</v>
@@ -2299,8 +2378,10 @@
 </v>
       </c>
       <c r="K42" t="str">
-        <f>CONCATENATE("case ", H42,  ": return ", C42, " (state, ", IF(F42="I", "rs, rt, imm", IF(F42="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 16: return MFHI (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H42, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C42,CHAR(34), "\n",");}",CHAR(10),"return ",C42," (state, ",IF(F42="I","rs, rt, imm",IF(F42="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 16:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MFHI"\n);}
+return MFHI (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>136</v>
@@ -2335,8 +2416,10 @@
 </v>
       </c>
       <c r="K43" t="str">
-        <f>CONCATENATE("case ", H43,  ": return ", C43, " (state, ", IF(F43="I", "rs, rt, imm", IF(F43="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 17: return MTHI (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H43, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C43,CHAR(34), "\n",");}",CHAR(10),"return ",C43," (state, ",IF(F43="I","rs, rt, imm",IF(F43="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 17:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MTHI"\n);}
+return MTHI (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>136</v>
@@ -2371,8 +2454,10 @@
 </v>
       </c>
       <c r="K44" t="str">
-        <f>CONCATENATE("case ", H44,  ": return ", C44, " (state, ", IF(F44="I", "rs, rt, imm", IF(F44="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 18: return MFLO (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H44, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C44,CHAR(34), "\n",");}",CHAR(10),"return ",C44," (state, ",IF(F44="I","rs, rt, imm",IF(F44="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 18:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MFLO"\n);}
+return MFLO (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>136</v>
@@ -2407,8 +2492,10 @@
 </v>
       </c>
       <c r="K45" t="str">
-        <f>CONCATENATE("case ", H45,  ": return ", C45, " (state, ", IF(F45="I", "rs, rt, imm", IF(F45="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 19: return MTLO (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H45, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C45,CHAR(34), "\n",");}",CHAR(10),"return ",C45," (state, ",IF(F45="I","rs, rt, imm",IF(F45="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 19:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MTLO"\n);}
+return MTLO (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>136</v>
@@ -2443,8 +2530,10 @@
 </v>
       </c>
       <c r="K46" t="str">
-        <f>CONCATENATE("case ", H46,  ": return ", C46, " (state, ", IF(F46="I", "rs, rt, imm", IF(F46="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 25: return MULTU (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H46, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C46,CHAR(34), "\n",");}",CHAR(10),"return ",C46," (state, ",IF(F46="I","rs, rt, imm",IF(F46="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 25:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MULTU"\n);}
+return MULTU (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L46" s="8" t="s">
         <v>136</v>
@@ -2479,8 +2568,10 @@
 </v>
       </c>
       <c r="K47" t="str">
-        <f>CONCATENATE("case ", H47,  ": return ", C47, " (state, ", IF(F47="I", "rs, rt, imm", IF(F47="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 27: return DIVU (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H47, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C47,CHAR(34), "\n",");}",CHAR(10),"return ",C47," (state, ",IF(F47="I","rs, rt, imm",IF(F47="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 27:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "DIVU"\n);}
+return DIVU (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L47" s="8" t="s">
         <v>136</v>
@@ -2517,8 +2608,10 @@
 </v>
       </c>
       <c r="K48" t="str">
-        <f>CONCATENATE("case ", H48,  ": return ", C48, " (state, ", IF(F48="I", "rs, rt, imm", IF(F48="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 1: return BLTZAL (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H48, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C48,CHAR(34), "\n",");}",CHAR(10),"return ",C48," (state, ",IF(F48="I","rs, rt, imm",IF(F48="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 1:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BLTZAL"\n);}
+return BLTZAL (state, rs, rt, imm);</v>
       </c>
       <c r="L48" s="8" t="s">
         <v>136</v>
@@ -2555,8 +2648,10 @@
 </v>
       </c>
       <c r="K49" t="str">
-        <f>CONCATENATE("case ", H49,  ": return ", C49, " (state, ", IF(F49="I", "rs, rt, imm", IF(F49="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 1: return BGEZAL (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H49, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C49,CHAR(34), "\n",");}",CHAR(10),"return ",C49," (state, ",IF(F49="I","rs, rt, imm",IF(F49="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 1:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "BGEZAL"\n);}
+return BGEZAL (state, rs, rt, imm);</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>136</v>
@@ -2591,8 +2686,10 @@
 </v>
       </c>
       <c r="K50" t="str">
-        <f>CONCATENATE("case ", H50,  ": return ", C50, " (state, ", IF(F50="I", "rs, rt, imm", IF(F50="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 3: return JAL (state,  target);</v>
+        <f>CONCATENATE("case ",H50, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C50,CHAR(34), "\n",");}",CHAR(10),"return ",C50," (state, ",IF(F50="I","rs, rt, imm",IF(F50="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 3:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "JAL"\n);}
+return JAL (state,  target);</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>136</v>
@@ -2627,8 +2724,10 @@
 </v>
       </c>
       <c r="K51" t="str">
-        <f>CONCATENATE("case ", H51,  ": return ", C51, " (state, ", IF(F51="I", "rs, rt, imm", IF(F51="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 9: return JALR (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H51, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C51,CHAR(34), "\n",");}",CHAR(10),"return ",C51," (state, ",IF(F51="I","rs, rt, imm",IF(F51="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 9:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "JALR"\n);}
+return JALR (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L51" s="8" t="s">
         <v>136</v>
@@ -2663,8 +2762,10 @@
 </v>
       </c>
       <c r="K52" t="str">
-        <f>CONCATENATE("case ", H52,  ": return ", C52, " (state, ", IF(F52="I", "rs, rt, imm", IF(F52="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 24: return MULT (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H52, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C52,CHAR(34), "\n",");}",CHAR(10),"return ",C52," (state, ",IF(F52="I","rs, rt, imm",IF(F52="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 24:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "MULT"\n);}
+return MULT (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>136</v>
@@ -2699,8 +2800,10 @@
 </v>
       </c>
       <c r="K53" t="str">
-        <f>CONCATENATE("case ", H53,  ": return ", C53, " (state, ", IF(F53="I", "rs, rt, imm", IF(F53="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 26: return DIV (state, rs, rt, rd, sa, function);</v>
+        <f>CONCATENATE("case ",H53, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C53,CHAR(34), "\n",");}",CHAR(10),"return ",C53," (state, ",IF(F53="I","rs, rt, imm",IF(F53="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 26:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "DIV"\n);}
+return DIV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L53" s="8" t="s">
         <v>136</v>
@@ -2735,8 +2838,10 @@
 </v>
       </c>
       <c r="K54" t="str">
-        <f>CONCATENATE("case ", H54,  ": return ", C54, " (state, ", IF(F54="I", "rs, rt, imm", IF(F54="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 34: return LWL (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H54, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C54,CHAR(34), "\n",");}",CHAR(10),"return ",C54," (state, ",IF(F54="I","rs, rt, imm",IF(F54="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 34:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LWL"\n);}
+return LWL (state, rs, rt, imm);</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>136</v>
@@ -2771,8 +2876,10 @@
 </v>
       </c>
       <c r="K55" t="str">
-        <f>CONCATENATE("case ", H55,  ": return ", C55, " (state, ", IF(F55="I", "rs, rt, imm", IF(F55="J", " target", "rs, rt, rd, sa, function")), ");")</f>
-        <v>case 38: return LWR (state, rs, rt, imm);</v>
+        <f>CONCATENATE("case ",H55, ":", CHAR(10),"if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, ",CHAR(34),C55,CHAR(34), "\n",");}",CHAR(10),"return ",C55," (state, ",IF(F55="I","rs, rt, imm",IF(F55="J"," target","rs, rt, rd, sa, function")),");")</f>
+        <v>case 38:
+if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "LWR"\n);}
+return LWR (state, rs, rt, imm);</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
+instr up to 2XX
</commit_message>
<xml_diff>
--- a/Instruction List.xlsx
+++ b/Instruction List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +463,14 @@
       <color rgb="FF333333"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -512,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -540,21 +548,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -853,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,7 +1354,7 @@
 return LUI (state, rs, rt, imm);</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1391,7 +1392,7 @@
 return LW (state, rs, rt, imm);</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1429,7 +1430,7 @@
 return SW (state, rs, rt, imm);</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1467,7 +1468,7 @@
 return SLL (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1505,7 +1506,7 @@
 return SRL (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1543,7 +1544,7 @@
 return SRA (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1581,7 +1582,7 @@
 return SRLV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1619,7 +1620,7 @@
 return SRAV (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1733,7 +1734,7 @@
 return SLT (state, rs, rt, rd, sa, function);</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1770,8 +1771,8 @@
 if(state-&gt;debug_level &gt; 0){fprintf(state-&gt;debug_out, "SLLV"\n);}
 return SLLV (state, rs, rt, rd, sa, function);</v>
       </c>
-      <c r="L25" s="8" t="s">
-        <v>136</v>
+      <c r="L25" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2137,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" ref="H35:H66" si="3">HEX2DEC(G35)</f>
+        <f t="shared" ref="H35:H55" si="3">HEX2DEC(G35)</f>
         <v>33</v>
       </c>
       <c r="I35" s="5"/>
@@ -2940,10 +2941,10 @@
     <sortCondition ref="I3:I55"/>
   </sortState>
   <conditionalFormatting sqref="L3:L55">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",L3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",L3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>